<commit_message>
Avance limpieza base de datos slack
</commit_message>
<xml_diff>
--- a/Krino-Slack/testslack.xlsx
+++ b/Krino-Slack/testslack.xlsx
@@ -882,12 +882,8 @@
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="inlineStr"/>
     </row>
@@ -1144,18 +1140,10 @@
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI7" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1437,18 +1425,12 @@
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI10" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1730,12 +1712,8 @@
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG13" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="inlineStr"/>
     </row>
@@ -1845,12 +1823,8 @@
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr"/>
       <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG14" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
       <c r="AI14" t="inlineStr"/>
     </row>
@@ -2569,12 +2543,8 @@
       <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG22" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr"/>
       <c r="AI22" t="inlineStr"/>
     </row>
@@ -2945,18 +2915,12 @@
       <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="inlineStr"/>
       <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF26" t="inlineStr"/>
       <c r="AG26" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH26" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI26" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -3923,12 +3887,8 @@
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="inlineStr"/>
-      <c r="AF37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG37" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="inlineStr"/>
       <c r="AH37" t="inlineStr"/>
       <c r="AI37" t="inlineStr"/>
     </row>
@@ -4125,12 +4085,8 @@
       <c r="AC39" t="inlineStr"/>
       <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="inlineStr"/>
-      <c r="AF39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG39" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="inlineStr"/>
       <c r="AH39" t="inlineStr"/>
       <c r="AI39" t="inlineStr"/>
     </row>
@@ -4762,18 +4718,12 @@
       <c r="AC46" t="inlineStr"/>
       <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="inlineStr"/>
-      <c r="AF46" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI46" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH46" t="inlineStr"/>
+      <c r="AI46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -5428,18 +5378,12 @@
       <c r="AC53" t="inlineStr"/>
       <c r="AD53" t="inlineStr"/>
       <c r="AE53" t="inlineStr"/>
-      <c r="AF53" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF53" t="inlineStr"/>
       <c r="AG53" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH53" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI53" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -5701,12 +5645,8 @@
       <c r="AC56" t="inlineStr"/>
       <c r="AD56" t="inlineStr"/>
       <c r="AE56" t="inlineStr"/>
-      <c r="AF56" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG56" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
       <c r="AH56" t="inlineStr"/>
       <c r="AI56" t="inlineStr"/>
     </row>
@@ -5899,12 +5839,8 @@
       <c r="AC58" t="inlineStr"/>
       <c r="AD58" t="inlineStr"/>
       <c r="AE58" t="inlineStr"/>
-      <c r="AF58" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG58" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF58" t="inlineStr"/>
+      <c r="AG58" t="inlineStr"/>
       <c r="AH58" t="inlineStr"/>
       <c r="AI58" t="inlineStr"/>
     </row>
@@ -6342,15 +6278,11 @@
       <c r="AC63" t="inlineStr"/>
       <c r="AD63" t="inlineStr"/>
       <c r="AE63" t="inlineStr"/>
-      <c r="AF63" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF63" t="inlineStr"/>
       <c r="AG63" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH63" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH63" t="inlineStr"/>
       <c r="AI63" t="inlineStr"/>
     </row>
     <row r="64">
@@ -6550,12 +6482,8 @@
       <c r="AC65" t="inlineStr"/>
       <c r="AD65" t="inlineStr"/>
       <c r="AE65" t="inlineStr"/>
-      <c r="AF65" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG65" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF65" t="inlineStr"/>
+      <c r="AG65" t="inlineStr"/>
       <c r="AH65" t="inlineStr"/>
       <c r="AI65" t="inlineStr"/>
     </row>
@@ -7355,12 +7283,8 @@
       <c r="AC74" t="inlineStr"/>
       <c r="AD74" t="inlineStr"/>
       <c r="AE74" t="inlineStr"/>
-      <c r="AF74" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG74" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF74" t="inlineStr"/>
+      <c r="AG74" t="inlineStr"/>
       <c r="AH74" t="inlineStr"/>
       <c r="AI74" t="inlineStr"/>
     </row>
@@ -7537,12 +7461,8 @@
       <c r="AC76" t="inlineStr"/>
       <c r="AD76" t="inlineStr"/>
       <c r="AE76" t="inlineStr"/>
-      <c r="AF76" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG76" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF76" t="inlineStr"/>
+      <c r="AG76" t="inlineStr"/>
       <c r="AH76" t="inlineStr"/>
       <c r="AI76" t="inlineStr"/>
     </row>
@@ -7723,12 +7643,8 @@
       <c r="AC78" t="inlineStr"/>
       <c r="AD78" t="inlineStr"/>
       <c r="AE78" t="inlineStr"/>
-      <c r="AF78" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG78" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF78" t="inlineStr"/>
+      <c r="AG78" t="inlineStr"/>
       <c r="AH78" t="inlineStr"/>
       <c r="AI78" t="inlineStr"/>
     </row>
@@ -8431,12 +8347,8 @@
       <c r="AC86" t="inlineStr"/>
       <c r="AD86" t="inlineStr"/>
       <c r="AE86" t="inlineStr"/>
-      <c r="AF86" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG86" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF86" t="inlineStr"/>
+      <c r="AG86" t="inlineStr"/>
       <c r="AH86" t="inlineStr"/>
       <c r="AI86" t="inlineStr"/>
     </row>
@@ -9859,12 +9771,8 @@
         </is>
       </c>
       <c r="AE103" t="inlineStr"/>
-      <c r="AF103" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG103" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF103" t="inlineStr"/>
+      <c r="AG103" t="inlineStr"/>
       <c r="AH103" t="inlineStr"/>
       <c r="AI103" t="inlineStr"/>
     </row>
@@ -10435,12 +10343,8 @@
       <c r="AC111" t="inlineStr"/>
       <c r="AD111" t="inlineStr"/>
       <c r="AE111" t="inlineStr"/>
-      <c r="AF111" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG111" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF111" t="inlineStr"/>
+      <c r="AG111" t="inlineStr"/>
       <c r="AH111" t="inlineStr"/>
       <c r="AI111" t="inlineStr"/>
     </row>
@@ -10708,12 +10612,8 @@
       <c r="AC114" t="inlineStr"/>
       <c r="AD114" t="inlineStr"/>
       <c r="AE114" t="inlineStr"/>
-      <c r="AF114" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG114" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF114" t="inlineStr"/>
+      <c r="AG114" t="inlineStr"/>
       <c r="AH114" t="inlineStr"/>
       <c r="AI114" t="inlineStr"/>
     </row>
@@ -10874,12 +10774,8 @@
       <c r="AC116" t="inlineStr"/>
       <c r="AD116" t="inlineStr"/>
       <c r="AE116" t="inlineStr"/>
-      <c r="AF116" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG116" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF116" t="inlineStr"/>
+      <c r="AG116" t="inlineStr"/>
       <c r="AH116" t="inlineStr"/>
       <c r="AI116" t="inlineStr"/>
     </row>
@@ -11147,12 +11043,8 @@
       <c r="AC119" t="inlineStr"/>
       <c r="AD119" t="inlineStr"/>
       <c r="AE119" t="inlineStr"/>
-      <c r="AF119" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG119" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF119" t="inlineStr"/>
+      <c r="AG119" t="inlineStr"/>
       <c r="AH119" t="inlineStr"/>
       <c r="AI119" t="inlineStr"/>
     </row>
@@ -11511,15 +11403,11 @@
       <c r="AC123" t="inlineStr"/>
       <c r="AD123" t="inlineStr"/>
       <c r="AE123" t="inlineStr"/>
-      <c r="AF123" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF123" t="inlineStr"/>
       <c r="AG123" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH123" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH123" t="inlineStr"/>
       <c r="AI123" t="inlineStr"/>
     </row>
     <row r="124">
@@ -11715,18 +11603,12 @@
       <c r="AC125" t="inlineStr"/>
       <c r="AD125" t="inlineStr"/>
       <c r="AE125" t="inlineStr"/>
-      <c r="AF125" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF125" t="inlineStr"/>
       <c r="AG125" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH125" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI125" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH125" t="inlineStr"/>
+      <c r="AI125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -12302,18 +12184,12 @@
       <c r="AC132" t="inlineStr"/>
       <c r="AD132" t="inlineStr"/>
       <c r="AE132" t="inlineStr"/>
-      <c r="AF132" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF132" t="inlineStr"/>
       <c r="AG132" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH132" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI132" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH132" t="inlineStr"/>
+      <c r="AI132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -12397,15 +12273,9 @@
       <c r="AC133" t="inlineStr"/>
       <c r="AD133" t="inlineStr"/>
       <c r="AE133" t="inlineStr"/>
-      <c r="AF133" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG133" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH133" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF133" t="inlineStr"/>
+      <c r="AG133" t="inlineStr"/>
+      <c r="AH133" t="inlineStr"/>
       <c r="AI133" t="inlineStr"/>
     </row>
     <row r="134">
@@ -12747,15 +12617,11 @@
       <c r="AC137" t="inlineStr"/>
       <c r="AD137" t="inlineStr"/>
       <c r="AE137" t="inlineStr"/>
-      <c r="AF137" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF137" t="inlineStr"/>
       <c r="AG137" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH137" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH137" t="inlineStr"/>
       <c r="AI137" t="inlineStr"/>
     </row>
     <row r="138">
@@ -12860,18 +12726,12 @@
       <c r="AC138" t="inlineStr"/>
       <c r="AD138" t="inlineStr"/>
       <c r="AE138" t="inlineStr"/>
-      <c r="AF138" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF138" t="inlineStr"/>
       <c r="AG138" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH138" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI138" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH138" t="inlineStr"/>
+      <c r="AI138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -12951,15 +12811,11 @@
       <c r="AC139" t="inlineStr"/>
       <c r="AD139" t="inlineStr"/>
       <c r="AE139" t="inlineStr"/>
-      <c r="AF139" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF139" t="inlineStr"/>
       <c r="AG139" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH139" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH139" t="inlineStr"/>
       <c r="AI139" t="inlineStr"/>
     </row>
     <row r="140">
@@ -13572,12 +13428,8 @@
       <c r="AC146" t="inlineStr"/>
       <c r="AD146" t="inlineStr"/>
       <c r="AE146" t="inlineStr"/>
-      <c r="AF146" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG146" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF146" t="inlineStr"/>
+      <c r="AG146" t="inlineStr"/>
       <c r="AH146" t="inlineStr"/>
       <c r="AI146" t="inlineStr"/>
     </row>
@@ -13861,18 +13713,12 @@
       <c r="AC149" t="inlineStr"/>
       <c r="AD149" t="inlineStr"/>
       <c r="AE149" t="inlineStr"/>
-      <c r="AF149" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF149" t="inlineStr"/>
       <c r="AG149" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH149" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI149" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH149" t="inlineStr"/>
+      <c r="AI149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -14695,12 +14541,8 @@
       <c r="AC159" t="inlineStr"/>
       <c r="AD159" t="inlineStr"/>
       <c r="AE159" t="inlineStr"/>
-      <c r="AF159" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG159" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF159" t="inlineStr"/>
+      <c r="AG159" t="inlineStr"/>
       <c r="AH159" t="inlineStr"/>
       <c r="AI159" t="inlineStr"/>
     </row>
@@ -14901,18 +14743,14 @@
       <c r="AC161" t="inlineStr"/>
       <c r="AD161" t="inlineStr"/>
       <c r="AE161" t="inlineStr"/>
-      <c r="AF161" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF161" t="inlineStr"/>
       <c r="AG161" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH161" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI161" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AI161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -15718,18 +15556,12 @@
       <c r="AC170" t="inlineStr"/>
       <c r="AD170" t="inlineStr"/>
       <c r="AE170" t="inlineStr"/>
-      <c r="AF170" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF170" t="inlineStr"/>
       <c r="AG170" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH170" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI170" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH170" t="inlineStr"/>
+      <c r="AI170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -16007,18 +15839,12 @@
       <c r="AC173" t="inlineStr"/>
       <c r="AD173" t="inlineStr"/>
       <c r="AE173" t="inlineStr"/>
-      <c r="AF173" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF173" t="inlineStr"/>
       <c r="AG173" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH173" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI173" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH173" t="inlineStr"/>
+      <c r="AI173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -16363,12 +16189,8 @@
       <c r="AC177" t="inlineStr"/>
       <c r="AD177" t="inlineStr"/>
       <c r="AE177" t="inlineStr"/>
-      <c r="AF177" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG177" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF177" t="inlineStr"/>
+      <c r="AG177" t="inlineStr"/>
       <c r="AH177" t="inlineStr"/>
       <c r="AI177" t="inlineStr"/>
     </row>
@@ -16482,15 +16304,9 @@
       <c r="AC178" t="inlineStr"/>
       <c r="AD178" t="inlineStr"/>
       <c r="AE178" t="inlineStr"/>
-      <c r="AF178" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG178" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH178" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF178" t="inlineStr"/>
+      <c r="AG178" t="inlineStr"/>
+      <c r="AH178" t="inlineStr"/>
       <c r="AI178" t="inlineStr"/>
     </row>
     <row r="179">
@@ -17535,12 +17351,8 @@
       <c r="AC190" t="inlineStr"/>
       <c r="AD190" t="inlineStr"/>
       <c r="AE190" t="inlineStr"/>
-      <c r="AF190" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG190" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF190" t="inlineStr"/>
+      <c r="AG190" t="inlineStr"/>
       <c r="AH190" t="inlineStr"/>
       <c r="AI190" t="inlineStr"/>
     </row>
@@ -17631,12 +17443,8 @@
       <c r="AC191" t="inlineStr"/>
       <c r="AD191" t="inlineStr"/>
       <c r="AE191" t="inlineStr"/>
-      <c r="AF191" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG191" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF191" t="inlineStr"/>
+      <c r="AG191" t="inlineStr"/>
       <c r="AH191" t="inlineStr"/>
       <c r="AI191" t="inlineStr"/>
     </row>
@@ -18066,12 +17874,8 @@
       <c r="AC196" t="inlineStr"/>
       <c r="AD196" t="inlineStr"/>
       <c r="AE196" t="inlineStr"/>
-      <c r="AF196" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG196" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF196" t="inlineStr"/>
+      <c r="AG196" t="inlineStr"/>
       <c r="AH196" t="inlineStr"/>
       <c r="AI196" t="inlineStr"/>
     </row>
@@ -19126,12 +18930,8 @@
       <c r="AC208" t="inlineStr"/>
       <c r="AD208" t="inlineStr"/>
       <c r="AE208" t="inlineStr"/>
-      <c r="AF208" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG208" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF208" t="inlineStr"/>
+      <c r="AG208" t="inlineStr"/>
       <c r="AH208" t="inlineStr"/>
       <c r="AI208" t="inlineStr"/>
     </row>
@@ -19395,12 +19195,8 @@
       <c r="AC211" t="inlineStr"/>
       <c r="AD211" t="inlineStr"/>
       <c r="AE211" t="inlineStr"/>
-      <c r="AF211" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG211" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF211" t="inlineStr"/>
+      <c r="AG211" t="inlineStr"/>
       <c r="AH211" t="inlineStr"/>
       <c r="AI211" t="inlineStr"/>
     </row>
@@ -19666,12 +19462,8 @@
       <c r="AC214" t="inlineStr"/>
       <c r="AD214" t="inlineStr"/>
       <c r="AE214" t="inlineStr"/>
-      <c r="AF214" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG214" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF214" t="inlineStr"/>
+      <c r="AG214" t="inlineStr"/>
       <c r="AH214" t="inlineStr"/>
       <c r="AI214" t="inlineStr"/>
     </row>
@@ -19775,12 +19567,8 @@
       <c r="AC215" t="inlineStr"/>
       <c r="AD215" t="inlineStr"/>
       <c r="AE215" t="inlineStr"/>
-      <c r="AF215" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG215" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF215" t="inlineStr"/>
+      <c r="AG215" t="inlineStr"/>
       <c r="AH215" t="inlineStr"/>
       <c r="AI215" t="inlineStr"/>
     </row>
@@ -20219,12 +20007,8 @@
       <c r="AC220" t="inlineStr"/>
       <c r="AD220" t="inlineStr"/>
       <c r="AE220" t="inlineStr"/>
-      <c r="AF220" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG220" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF220" t="inlineStr"/>
+      <c r="AG220" t="inlineStr"/>
       <c r="AH220" t="inlineStr"/>
       <c r="AI220" t="inlineStr"/>
     </row>
@@ -20314,18 +20098,10 @@
       <c r="AC221" t="inlineStr"/>
       <c r="AD221" t="inlineStr"/>
       <c r="AE221" t="inlineStr"/>
-      <c r="AF221" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG221" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH221" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI221" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF221" t="inlineStr"/>
+      <c r="AG221" t="inlineStr"/>
+      <c r="AH221" t="inlineStr"/>
+      <c r="AI221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -20520,15 +20296,11 @@
       <c r="AC223" t="inlineStr"/>
       <c r="AD223" t="inlineStr"/>
       <c r="AE223" t="inlineStr"/>
-      <c r="AF223" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF223" t="inlineStr"/>
       <c r="AG223" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH223" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH223" t="inlineStr"/>
       <c r="AI223" t="inlineStr"/>
     </row>
     <row r="224">
@@ -21318,12 +21090,8 @@
       <c r="AC232" t="inlineStr"/>
       <c r="AD232" t="inlineStr"/>
       <c r="AE232" t="inlineStr"/>
-      <c r="AF232" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG232" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF232" t="inlineStr"/>
+      <c r="AG232" t="inlineStr"/>
       <c r="AH232" t="inlineStr"/>
       <c r="AI232" t="inlineStr"/>
     </row>
@@ -21500,12 +21268,8 @@
       <c r="AC234" t="inlineStr"/>
       <c r="AD234" t="inlineStr"/>
       <c r="AE234" t="inlineStr"/>
-      <c r="AF234" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG234" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF234" t="inlineStr"/>
+      <c r="AG234" t="inlineStr"/>
       <c r="AH234" t="inlineStr"/>
       <c r="AI234" t="inlineStr"/>
     </row>
@@ -22131,12 +21895,8 @@
       <c r="AC241" t="inlineStr"/>
       <c r="AD241" t="inlineStr"/>
       <c r="AE241" t="inlineStr"/>
-      <c r="AF241" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG241" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF241" t="inlineStr"/>
+      <c r="AG241" t="inlineStr"/>
       <c r="AH241" t="inlineStr"/>
       <c r="AI241" t="inlineStr"/>
     </row>
@@ -22566,12 +22326,8 @@
       <c r="AC246" t="inlineStr"/>
       <c r="AD246" t="inlineStr"/>
       <c r="AE246" t="inlineStr"/>
-      <c r="AF246" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG246" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF246" t="inlineStr"/>
+      <c r="AG246" t="inlineStr"/>
       <c r="AH246" t="inlineStr"/>
       <c r="AI246" t="inlineStr"/>
     </row>
@@ -22677,12 +22433,8 @@
       <c r="AC247" t="inlineStr"/>
       <c r="AD247" t="inlineStr"/>
       <c r="AE247" t="inlineStr"/>
-      <c r="AF247" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG247" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF247" t="inlineStr"/>
+      <c r="AG247" t="inlineStr"/>
       <c r="AH247" t="inlineStr"/>
       <c r="AI247" t="inlineStr"/>
     </row>
@@ -22859,12 +22611,8 @@
       <c r="AC249" t="inlineStr"/>
       <c r="AD249" t="inlineStr"/>
       <c r="AE249" t="inlineStr"/>
-      <c r="AF249" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG249" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF249" t="inlineStr"/>
+      <c r="AG249" t="inlineStr"/>
       <c r="AH249" t="inlineStr"/>
       <c r="AI249" t="inlineStr"/>
     </row>
@@ -22955,12 +22703,8 @@
       <c r="AC250" t="inlineStr"/>
       <c r="AD250" t="inlineStr"/>
       <c r="AE250" t="inlineStr"/>
-      <c r="AF250" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG250" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF250" t="inlineStr"/>
+      <c r="AG250" t="inlineStr"/>
       <c r="AH250" t="inlineStr"/>
       <c r="AI250" t="inlineStr"/>
     </row>
@@ -23050,12 +22794,8 @@
       <c r="AC251" t="inlineStr"/>
       <c r="AD251" t="inlineStr"/>
       <c r="AE251" t="inlineStr"/>
-      <c r="AF251" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG251" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF251" t="inlineStr"/>
+      <c r="AG251" t="inlineStr"/>
       <c r="AH251" t="inlineStr"/>
       <c r="AI251" t="inlineStr"/>
     </row>
@@ -23778,12 +23518,8 @@
       <c r="AC259" t="inlineStr"/>
       <c r="AD259" t="inlineStr"/>
       <c r="AE259" t="inlineStr"/>
-      <c r="AF259" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG259" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF259" t="inlineStr"/>
+      <c r="AG259" t="inlineStr"/>
       <c r="AH259" t="inlineStr"/>
       <c r="AI259" t="inlineStr"/>
     </row>
@@ -23960,12 +23696,8 @@
       <c r="AC261" t="inlineStr"/>
       <c r="AD261" t="inlineStr"/>
       <c r="AE261" t="inlineStr"/>
-      <c r="AF261" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG261" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF261" t="inlineStr"/>
+      <c r="AG261" t="inlineStr"/>
       <c r="AH261" t="inlineStr"/>
       <c r="AI261" t="inlineStr"/>
     </row>
@@ -24063,12 +23795,8 @@
       <c r="AC262" t="inlineStr"/>
       <c r="AD262" t="inlineStr"/>
       <c r="AE262" t="inlineStr"/>
-      <c r="AF262" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG262" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF262" t="inlineStr"/>
+      <c r="AG262" t="inlineStr"/>
       <c r="AH262" t="inlineStr"/>
       <c r="AI262" t="inlineStr"/>
     </row>
@@ -24263,15 +23991,11 @@
       <c r="AC264" t="inlineStr"/>
       <c r="AD264" t="inlineStr"/>
       <c r="AE264" t="inlineStr"/>
-      <c r="AF264" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF264" t="inlineStr"/>
       <c r="AG264" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH264" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH264" t="inlineStr"/>
       <c r="AI264" t="inlineStr"/>
     </row>
     <row r="265">
@@ -24544,15 +24268,11 @@
       <c r="AC267" t="inlineStr"/>
       <c r="AD267" t="inlineStr"/>
       <c r="AE267" t="inlineStr"/>
-      <c r="AF267" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF267" t="inlineStr"/>
       <c r="AG267" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH267" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH267" t="inlineStr"/>
       <c r="AI267" t="inlineStr"/>
     </row>
     <row r="268">
@@ -24740,15 +24460,11 @@
       <c r="AC269" t="inlineStr"/>
       <c r="AD269" t="inlineStr"/>
       <c r="AE269" t="inlineStr"/>
-      <c r="AF269" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF269" t="inlineStr"/>
       <c r="AG269" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH269" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH269" t="inlineStr"/>
       <c r="AI269" t="inlineStr"/>
     </row>
     <row r="270">
@@ -24850,15 +24566,9 @@
       <c r="AC270" t="inlineStr"/>
       <c r="AD270" t="inlineStr"/>
       <c r="AE270" t="inlineStr"/>
-      <c r="AF270" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG270" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH270" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF270" t="inlineStr"/>
+      <c r="AG270" t="inlineStr"/>
+      <c r="AH270" t="inlineStr"/>
       <c r="AI270" t="inlineStr"/>
     </row>
     <row r="271">
@@ -24947,12 +24657,8 @@
       <c r="AC271" t="inlineStr"/>
       <c r="AD271" t="inlineStr"/>
       <c r="AE271" t="inlineStr"/>
-      <c r="AF271" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG271" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF271" t="inlineStr"/>
+      <c r="AG271" t="inlineStr"/>
       <c r="AH271" t="inlineStr"/>
       <c r="AI271" t="inlineStr"/>
     </row>
@@ -25660,12 +25366,8 @@
       <c r="AC279" t="inlineStr"/>
       <c r="AD279" t="inlineStr"/>
       <c r="AE279" t="inlineStr"/>
-      <c r="AF279" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG279" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF279" t="inlineStr"/>
+      <c r="AG279" t="inlineStr"/>
       <c r="AH279" t="inlineStr"/>
       <c r="AI279" t="inlineStr"/>
     </row>
@@ -27036,12 +26738,8 @@
       <c r="AC295" t="inlineStr"/>
       <c r="AD295" t="inlineStr"/>
       <c r="AE295" t="inlineStr"/>
-      <c r="AF295" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG295" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF295" t="inlineStr"/>
+      <c r="AG295" t="inlineStr"/>
       <c r="AH295" t="inlineStr"/>
       <c r="AI295" t="inlineStr"/>
     </row>
@@ -27408,15 +27106,9 @@
       <c r="AC299" t="inlineStr"/>
       <c r="AD299" t="inlineStr"/>
       <c r="AE299" t="inlineStr"/>
-      <c r="AF299" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG299" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH299" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF299" t="inlineStr"/>
+      <c r="AG299" t="inlineStr"/>
+      <c r="AH299" t="inlineStr"/>
       <c r="AI299" t="inlineStr"/>
     </row>
     <row r="300">
@@ -27521,15 +27213,9 @@
       <c r="AC300" t="inlineStr"/>
       <c r="AD300" t="inlineStr"/>
       <c r="AE300" t="inlineStr"/>
-      <c r="AF300" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG300" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH300" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF300" t="inlineStr"/>
+      <c r="AG300" t="inlineStr"/>
+      <c r="AH300" t="inlineStr"/>
       <c r="AI300" t="inlineStr"/>
     </row>
     <row r="301">
@@ -28006,12 +27692,8 @@
       <c r="AC305" t="inlineStr"/>
       <c r="AD305" t="inlineStr"/>
       <c r="AE305" t="inlineStr"/>
-      <c r="AF305" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG305" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF305" t="inlineStr"/>
+      <c r="AG305" t="inlineStr"/>
       <c r="AH305" t="inlineStr"/>
       <c r="AI305" t="inlineStr"/>
     </row>
@@ -28209,12 +27891,8 @@
       <c r="AC307" t="inlineStr"/>
       <c r="AD307" t="inlineStr"/>
       <c r="AE307" t="inlineStr"/>
-      <c r="AF307" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG307" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF307" t="inlineStr"/>
+      <c r="AG307" t="inlineStr"/>
       <c r="AH307" t="inlineStr"/>
       <c r="AI307" t="inlineStr"/>
     </row>
@@ -28324,18 +28002,12 @@
       <c r="AC308" t="inlineStr"/>
       <c r="AD308" t="inlineStr"/>
       <c r="AE308" t="inlineStr"/>
-      <c r="AF308" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF308" t="inlineStr"/>
       <c r="AG308" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH308" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI308" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH308" t="inlineStr"/>
+      <c r="AI308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -28435,18 +28107,12 @@
       <c r="AC309" t="inlineStr"/>
       <c r="AD309" t="inlineStr"/>
       <c r="AE309" t="inlineStr"/>
-      <c r="AF309" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF309" t="inlineStr"/>
       <c r="AG309" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH309" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI309" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH309" t="inlineStr"/>
+      <c r="AI309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -28815,15 +28481,9 @@
       <c r="AC313" t="inlineStr"/>
       <c r="AD313" t="inlineStr"/>
       <c r="AE313" t="inlineStr"/>
-      <c r="AF313" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG313" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH313" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF313" t="inlineStr"/>
+      <c r="AG313" t="inlineStr"/>
+      <c r="AH313" t="inlineStr"/>
       <c r="AI313" t="inlineStr"/>
     </row>
     <row r="314">
@@ -28999,12 +28659,8 @@
       <c r="AC315" t="inlineStr"/>
       <c r="AD315" t="inlineStr"/>
       <c r="AE315" t="inlineStr"/>
-      <c r="AF315" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG315" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF315" t="inlineStr"/>
+      <c r="AG315" t="inlineStr"/>
       <c r="AH315" t="inlineStr"/>
       <c r="AI315" t="inlineStr"/>
     </row>
@@ -29094,12 +28750,8 @@
       <c r="AC316" t="inlineStr"/>
       <c r="AD316" t="inlineStr"/>
       <c r="AE316" t="inlineStr"/>
-      <c r="AF316" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG316" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF316" t="inlineStr"/>
+      <c r="AG316" t="inlineStr"/>
       <c r="AH316" t="inlineStr"/>
       <c r="AI316" t="inlineStr"/>
     </row>
@@ -29369,18 +29021,12 @@
       <c r="AC319" t="inlineStr"/>
       <c r="AD319" t="inlineStr"/>
       <c r="AE319" t="inlineStr"/>
-      <c r="AF319" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF319" t="inlineStr"/>
       <c r="AG319" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH319" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI319" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH319" t="inlineStr"/>
+      <c r="AI319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -29488,18 +29134,12 @@
       <c r="AC320" t="inlineStr"/>
       <c r="AD320" t="inlineStr"/>
       <c r="AE320" t="inlineStr"/>
-      <c r="AF320" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF320" t="inlineStr"/>
       <c r="AG320" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH320" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI320" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH320" t="inlineStr"/>
+      <c r="AI320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -30379,18 +30019,12 @@
       <c r="AC330" t="inlineStr"/>
       <c r="AD330" t="inlineStr"/>
       <c r="AE330" t="inlineStr"/>
-      <c r="AF330" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF330" t="inlineStr"/>
       <c r="AG330" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH330" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI330" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH330" t="inlineStr"/>
+      <c r="AI330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -30498,15 +30132,11 @@
       <c r="AC331" t="inlineStr"/>
       <c r="AD331" t="inlineStr"/>
       <c r="AE331" t="inlineStr"/>
-      <c r="AF331" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF331" t="inlineStr"/>
       <c r="AG331" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH331" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH331" t="inlineStr"/>
       <c r="AI331" t="inlineStr"/>
     </row>
     <row r="332">
@@ -30802,15 +30432,11 @@
       <c r="AC334" t="inlineStr"/>
       <c r="AD334" t="inlineStr"/>
       <c r="AE334" t="inlineStr"/>
-      <c r="AF334" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF334" t="inlineStr"/>
       <c r="AG334" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH334" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH334" t="inlineStr"/>
       <c r="AI334" t="inlineStr"/>
     </row>
     <row r="335">
@@ -30919,18 +30545,14 @@
       <c r="AC335" t="inlineStr"/>
       <c r="AD335" t="inlineStr"/>
       <c r="AE335" t="inlineStr"/>
-      <c r="AF335" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF335" t="inlineStr"/>
       <c r="AG335" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH335" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI335" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AI335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -32075,12 +31697,8 @@
       <c r="AC348" t="inlineStr"/>
       <c r="AD348" t="inlineStr"/>
       <c r="AE348" t="inlineStr"/>
-      <c r="AF348" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG348" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF348" t="inlineStr"/>
+      <c r="AG348" t="inlineStr"/>
       <c r="AH348" t="inlineStr"/>
       <c r="AI348" t="inlineStr"/>
     </row>
@@ -32344,12 +31962,8 @@
       <c r="AC351" t="inlineStr"/>
       <c r="AD351" t="inlineStr"/>
       <c r="AE351" t="inlineStr"/>
-      <c r="AF351" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG351" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF351" t="inlineStr"/>
+      <c r="AG351" t="inlineStr"/>
       <c r="AH351" t="inlineStr"/>
       <c r="AI351" t="inlineStr"/>
     </row>
@@ -32451,12 +32065,12 @@
       <c r="AC352" t="inlineStr"/>
       <c r="AD352" t="inlineStr"/>
       <c r="AE352" t="inlineStr"/>
-      <c r="AF352" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG352" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF352" t="inlineStr">
+        <is>
+          <t>['F02TCEZGZ45']</t>
+        </is>
+      </c>
+      <c r="AG352" t="inlineStr"/>
       <c r="AH352" t="inlineStr"/>
       <c r="AI352" t="inlineStr"/>
     </row>
@@ -32736,15 +32350,11 @@
       <c r="AC355" t="inlineStr"/>
       <c r="AD355" t="inlineStr"/>
       <c r="AE355" t="inlineStr"/>
-      <c r="AF355" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF355" t="inlineStr"/>
       <c r="AG355" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH355" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH355" t="inlineStr"/>
       <c r="AI355" t="inlineStr"/>
     </row>
     <row r="356">
@@ -32940,18 +32550,12 @@
       <c r="AC357" t="inlineStr"/>
       <c r="AD357" t="inlineStr"/>
       <c r="AE357" t="inlineStr"/>
-      <c r="AF357" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF357" t="inlineStr"/>
       <c r="AG357" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH357" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI357" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH357" t="inlineStr"/>
+      <c r="AI357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -33059,12 +32663,8 @@
       <c r="AC358" t="inlineStr"/>
       <c r="AD358" t="inlineStr"/>
       <c r="AE358" t="inlineStr"/>
-      <c r="AF358" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG358" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF358" t="inlineStr"/>
+      <c r="AG358" t="inlineStr"/>
       <c r="AH358" t="inlineStr"/>
       <c r="AI358" t="inlineStr"/>
     </row>
@@ -33344,15 +32944,11 @@
       <c r="AC361" t="inlineStr"/>
       <c r="AD361" t="inlineStr"/>
       <c r="AE361" t="inlineStr"/>
-      <c r="AF361" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF361" t="inlineStr"/>
       <c r="AG361" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH361" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH361" t="inlineStr"/>
       <c r="AI361" t="inlineStr"/>
     </row>
     <row r="362">
@@ -33457,18 +33053,12 @@
       <c r="AC362" t="inlineStr"/>
       <c r="AD362" t="inlineStr"/>
       <c r="AE362" t="inlineStr"/>
-      <c r="AF362" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF362" t="inlineStr"/>
       <c r="AG362" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH362" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI362" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH362" t="inlineStr"/>
+      <c r="AI362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -33576,15 +33166,9 @@
       <c r="AC363" t="inlineStr"/>
       <c r="AD363" t="inlineStr"/>
       <c r="AE363" t="inlineStr"/>
-      <c r="AF363" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG363" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH363" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF363" t="inlineStr"/>
+      <c r="AG363" t="inlineStr"/>
+      <c r="AH363" t="inlineStr"/>
       <c r="AI363" t="inlineStr"/>
     </row>
     <row r="364">
@@ -34282,12 +33866,8 @@
       <c r="AC371" t="inlineStr"/>
       <c r="AD371" t="inlineStr"/>
       <c r="AE371" t="inlineStr"/>
-      <c r="AF371" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG371" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF371" t="inlineStr"/>
+      <c r="AG371" t="inlineStr"/>
       <c r="AH371" t="inlineStr"/>
       <c r="AI371" t="inlineStr"/>
     </row>
@@ -34916,12 +34496,8 @@
       <c r="AC378" t="inlineStr"/>
       <c r="AD378" t="inlineStr"/>
       <c r="AE378" t="inlineStr"/>
-      <c r="AF378" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG378" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF378" t="inlineStr"/>
+      <c r="AG378" t="inlineStr"/>
       <c r="AH378" t="inlineStr"/>
       <c r="AI378" t="inlineStr"/>
     </row>
@@ -35023,18 +34599,10 @@
       <c r="AC379" t="inlineStr"/>
       <c r="AD379" t="inlineStr"/>
       <c r="AE379" t="inlineStr"/>
-      <c r="AF379" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG379" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH379" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI379" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF379" t="inlineStr"/>
+      <c r="AG379" t="inlineStr"/>
+      <c r="AH379" t="inlineStr"/>
+      <c r="AI379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
@@ -35395,15 +34963,9 @@
       <c r="AC383" t="inlineStr"/>
       <c r="AD383" t="inlineStr"/>
       <c r="AE383" t="inlineStr"/>
-      <c r="AF383" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG383" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH383" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF383" t="inlineStr"/>
+      <c r="AG383" t="inlineStr"/>
+      <c r="AH383" t="inlineStr"/>
       <c r="AI383" t="inlineStr"/>
     </row>
     <row r="384">
@@ -36019,12 +35581,8 @@
       <c r="AC390" t="inlineStr"/>
       <c r="AD390" t="inlineStr"/>
       <c r="AE390" t="inlineStr"/>
-      <c r="AF390" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG390" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF390" t="inlineStr"/>
+      <c r="AG390" t="inlineStr"/>
       <c r="AH390" t="inlineStr"/>
       <c r="AI390" t="inlineStr"/>
     </row>
@@ -36388,18 +35946,12 @@
       <c r="AC394" t="inlineStr"/>
       <c r="AD394" t="inlineStr"/>
       <c r="AE394" t="inlineStr"/>
-      <c r="AF394" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF394" t="inlineStr"/>
       <c r="AG394" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH394" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI394" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH394" t="inlineStr"/>
+      <c r="AI394" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
@@ -36594,18 +36146,12 @@
       <c r="AC396" t="inlineStr"/>
       <c r="AD396" t="inlineStr"/>
       <c r="AE396" t="inlineStr"/>
-      <c r="AF396" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF396" t="inlineStr"/>
       <c r="AG396" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH396" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI396" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH396" t="inlineStr"/>
+      <c r="AI396" t="inlineStr"/>
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
@@ -36974,15 +36520,9 @@
       <c r="AC400" t="inlineStr"/>
       <c r="AD400" t="inlineStr"/>
       <c r="AE400" t="inlineStr"/>
-      <c r="AF400" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG400" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH400" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF400" t="inlineStr"/>
+      <c r="AG400" t="inlineStr"/>
+      <c r="AH400" t="inlineStr"/>
       <c r="AI400" t="inlineStr"/>
     </row>
     <row r="401">
@@ -37257,15 +36797,11 @@
       <c r="AC403" t="inlineStr"/>
       <c r="AD403" t="inlineStr"/>
       <c r="AE403" t="inlineStr"/>
-      <c r="AF403" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF403" t="inlineStr"/>
       <c r="AG403" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH403" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH403" t="inlineStr"/>
       <c r="AI403" t="inlineStr"/>
     </row>
     <row r="404">
@@ -37809,15 +37345,9 @@
       <c r="AC409" t="inlineStr"/>
       <c r="AD409" t="inlineStr"/>
       <c r="AE409" t="inlineStr"/>
-      <c r="AF409" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG409" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH409" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF409" t="inlineStr"/>
+      <c r="AG409" t="inlineStr"/>
+      <c r="AH409" t="inlineStr"/>
       <c r="AI409" t="inlineStr"/>
     </row>
     <row r="410">
@@ -38526,15 +38056,11 @@
       <c r="AC417" t="inlineStr"/>
       <c r="AD417" t="inlineStr"/>
       <c r="AE417" t="inlineStr"/>
-      <c r="AF417" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF417" t="inlineStr"/>
       <c r="AG417" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH417" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH417" t="inlineStr"/>
       <c r="AI417" t="inlineStr"/>
     </row>
     <row r="418">
@@ -38996,18 +38522,12 @@
       <c r="AC422" t="inlineStr"/>
       <c r="AD422" t="inlineStr"/>
       <c r="AE422" t="inlineStr"/>
-      <c r="AF422" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF422" t="inlineStr"/>
       <c r="AG422" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH422" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI422" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AH422" t="inlineStr"/>
+      <c r="AI422" t="inlineStr"/>
     </row>
     <row r="423">
       <c r="A423" s="1" t="n">
@@ -39456,17 +38976,11 @@
       <c r="AC427" t="inlineStr"/>
       <c r="AD427" t="inlineStr"/>
       <c r="AE427" t="inlineStr"/>
-      <c r="AF427" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG427" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH427" t="b">
-        <v>0</v>
-      </c>
+      <c r="AF427" t="inlineStr"/>
+      <c r="AG427" t="inlineStr"/>
+      <c r="AH427" t="inlineStr"/>
       <c r="AI427" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428">

</xml_diff>